<commit_message>
Alteração da base de dados
Correção de erro de digitação
</commit_message>
<xml_diff>
--- a/SIMULADOR FII.xlsx
+++ b/SIMULADOR FII.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84704001185c0313/Documents/CURSO EXCEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84704001185c0313/Documents/CURSO EXCEL/GIT-GITHUB-DIU/planilha-fiis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="8_{3FA65942-C9DF-468E-B0EA-5568C7E8B34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C32A6120-63D0-4438-9CB5-DDB5299DC532}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="8_{3FA65942-C9DF-468E-B0EA-5568C7E8B34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8427FD3E-3A8B-4AC6-B04A-C7AE871DC37A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EB58D97-D116-4FEE-B598-F6572D0553C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6EB58D97-D116-4FEE-B598-F6572D0553C4}"/>
   </bookViews>
   <sheets>
     <sheet name="FIIs - Análise Investimeno" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t>Patrimônio acumulado:</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>TIJOLO</t>
-  </si>
-  <si>
-    <t>HÍBRIDOS</t>
   </si>
   <si>
     <t>FOFS</t>
@@ -165,8 +162,8 @@
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="173" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -971,134 +968,59 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="6" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
@@ -1115,54 +1037,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="7" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -1332,6 +1326,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1377,6 +1376,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1397,6 +1401,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1417,6 +1426,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1437,6 +1451,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1590,6 +1609,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1610,6 +1634,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1630,6 +1659,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1650,6 +1684,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1670,6 +1709,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1690,6 +1734,11 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-0E72-4568-826E-80876486584E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -3971,7 +4020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40130C33-4D69-4023-9FE0-85DE6757A8FE}">
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C80" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -3984,6 +4033,7 @@
     <col min="5" max="5" width="31.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -4000,151 +4050,140 @@
     <row r="11" spans="4:6" x14ac:dyDescent="0.25"/>
     <row r="12" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="73"/>
+      <c r="F13" s="74"/>
+    </row>
+    <row r="14" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="75"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="77"/>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="85"/>
+      <c r="F15" s="9">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="24">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D16" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="25">
+      <c r="E16" s="59"/>
+      <c r="F16" s="10">
         <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="26">
+      <c r="D17" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="57"/>
+      <c r="F17" s="11">
         <f>F15*30%</f>
         <v>1260</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D18" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="27">
+      <c r="D18" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="59"/>
+      <c r="F18" s="12">
         <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D19" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="28">
+      <c r="D19" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="59"/>
+      <c r="F19" s="13">
         <v>5</v>
       </c>
-      <c r="L19" s="10"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="29" t="s">
+      <c r="D20" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D22" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="7"/>
+      <c r="D22" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="79"/>
+      <c r="F22" s="80"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="22"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="7"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="38">
+      <c r="E24" s="63"/>
+      <c r="F24" s="15">
         <f>FV(tax_rendimento,prazo_anos*12,aporte)*-1</f>
         <v>114051.53941827051</v>
       </c>
-      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="39">
+      <c r="E25" s="65"/>
+      <c r="F25" s="16">
         <f>F24*tax_rendimento</f>
         <v>2281.03078836541</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="8"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="5"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="73" t="s">
+      <c r="D28" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="75" t="s">
+      <c r="E28" s="68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="70" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="76"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="78"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="71"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
-      <c r="D30" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="71">
+      <c r="D30" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="44">
         <f>FV(tax_rendimento,A30*12,aporte)*-1</f>
         <v>30421.862473761252</v>
       </c>
-      <c r="F30" s="72">
+      <c r="F30" s="45">
         <f>E30*tax_rendimento</f>
         <v>608.43724947522503</v>
       </c>
@@ -4153,14 +4192,14 @@
       <c r="A31">
         <v>5</v>
       </c>
-      <c r="D31" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="45">
+      <c r="D31" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="18">
         <f>FV(tax_rendimento,A31*12,aporte)*-1</f>
         <v>114051.53941827051</v>
       </c>
-      <c r="F31" s="46">
+      <c r="F31" s="19">
         <f>E31*tax_rendimento</f>
         <v>2281.03078836541</v>
       </c>
@@ -4169,14 +4208,14 @@
       <c r="A32">
         <v>10</v>
       </c>
-      <c r="D32" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="45">
+      <c r="D32" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="18">
         <f>FV(tax_rendimento,A32*12,aporte)*-1</f>
         <v>488258.15171008714</v>
       </c>
-      <c r="F32" s="46">
+      <c r="F32" s="19">
         <f>E32*tax_rendimento</f>
         <v>9765.1630342017434</v>
       </c>
@@ -4185,14 +4224,14 @@
       <c r="A33">
         <v>20</v>
       </c>
-      <c r="D33" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="45">
+      <c r="D33" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="18">
         <f>FV(tax_rendimento,A33*12,aporte)*-1</f>
         <v>5744436.7576471847</v>
       </c>
-      <c r="F33" s="46">
+      <c r="F33" s="19">
         <f>E33*tax_rendimento</f>
         <v>114888.7351529437</v>
       </c>
@@ -4201,226 +4240,146 @@
       <c r="A34">
         <v>30</v>
       </c>
-      <c r="D34" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="48">
+      <c r="D34" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="21">
         <f>FV(tax_rendimento,A34*12,aporte)*-1</f>
         <v>62328056.387443289</v>
       </c>
-      <c r="F34" s="49">
+      <c r="F34" s="22">
         <f>E34*tax_rendimento</f>
         <v>1246561.1277488659</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-    </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-    </row>
-    <row r="53" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D54" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="E54" s="85" t="s">
+      <c r="D54" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="23"/>
+      <c r="F54" s="8"/>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="E55" s="86">
+      <c r="D55" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="53">
         <f>aporte</f>
         <v>1000</v>
       </c>
-      <c r="F55" s="84"/>
+      <c r="F55" s="51"/>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="82" t="s">
+      <c r="D56" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" s="82" t="s">
-        <v>29</v>
+      <c r="E56" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="49" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D57" s="79" t="s">
+      <c r="D57" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="80">
+      <c r="E57" s="47">
         <f>VLOOKUP(perfil&amp;"-"&amp;D57,Perfis!$A:$D,4,)</f>
         <v>0.5</v>
       </c>
-      <c r="F57" s="81">
+      <c r="F57" s="48">
         <f>$E$55*E57</f>
         <v>500</v>
       </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D58" s="50" t="s">
+      <c r="D58" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="51">
+      <c r="E58" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D58,Perfis!$A:$D,4,)</f>
         <v>0.1</v>
       </c>
-      <c r="F58" s="81">
+      <c r="F58" s="48">
         <f t="shared" ref="F58:F62" si="0">$E$55*E58</f>
         <v>100</v>
       </c>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D59" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59" s="51">
+      <c r="D59" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D59,Perfis!$A:$D,4,)</f>
         <v>0.05</v>
       </c>
-      <c r="F59" s="81">
+      <c r="F59" s="48">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="51">
+      <c r="D60" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D60,Perfis!$A:$D,4,)</f>
         <v>0.05</v>
       </c>
-      <c r="F60" s="81">
+      <c r="F60" s="48">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D61" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="51">
+      <c r="D61" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D61,Perfis!$A:$D,4,)</f>
         <v>0.2</v>
       </c>
-      <c r="F61" s="81">
+      <c r="F61" s="48">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
     <row r="62" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="E62" s="69">
+      <c r="D62" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="42">
         <f>VLOOKUP(perfil&amp;"-"&amp;D62,Perfis!$A:$D,4,)</f>
         <v>0.1</v>
       </c>
-      <c r="F62" s="88">
+      <c r="F62" s="55">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="4:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-    </row>
+    <row r="63" spans="4:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="4:6" x14ac:dyDescent="0.25"/>
     <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4440,11 +4399,6 @@
     <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="E28:E29"/>
@@ -4453,6 +4407,11 @@
     <mergeCell ref="D22:F23"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D24:E24"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F20" xr:uid="{C12BE7FF-F9F6-4578-84C8-CEB316F83E59}">
@@ -4468,8 +4427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFA9F09-09B6-405B-A602-891185294CC5}">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4482,17 +4441,17 @@
   <sheetData>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="C3" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="60" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4500,13 +4459,13 @@
         <f t="shared" ref="A4:A21" si="0">B4&amp;"-"&amp;C4</f>
         <v>Conservador-PAPEL</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="38">
         <v>0.3</v>
       </c>
     </row>
@@ -4534,7 +4493,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4">
         <v>0.1</v>
@@ -4549,7 +4508,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4">
         <v>0.1</v>
@@ -4564,24 +4523,24 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="66" t="str">
+      <c r="A9" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-HOTELARIA</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="68">
+      <c r="C9" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="41">
         <v>0</v>
       </c>
     </row>
@@ -4590,13 +4549,13 @@
         <f t="shared" si="0"/>
         <v>Moderado-PAPEL</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="38">
         <v>0.32</v>
       </c>
     </row>
@@ -4618,13 +4577,13 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Moderado-HÍBRIDOS</v>
+        <v>Moderado-HIBRIDOS</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4">
         <v>0.08</v>
@@ -4639,7 +4598,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="4">
         <v>0.1</v>
@@ -4654,44 +4613,44 @@
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="4">
         <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="66" t="str">
+      <c r="A15" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-HOTELARIA</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="68">
+      <c r="C15" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="41">
         <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="str">
+      <c r="A16" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-PAPEL</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="63">
+      <c r="D16" s="36">
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="str">
+      <c r="A17" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-TIJOLO</v>
       </c>
@@ -4701,12 +4660,12 @@
       <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="27">
         <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="str">
+      <c r="A18" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-HIBRIDOS</v>
       </c>
@@ -4714,14 +4673,14 @@
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="54">
+        <v>19</v>
+      </c>
+      <c r="D18" s="27">
         <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="str">
+      <c r="A19" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-FOFS</v>
       </c>
@@ -4729,14 +4688,14 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="54">
+        <v>11</v>
+      </c>
+      <c r="D19" s="27">
         <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="str">
+      <c r="A20" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-DESENVOLVIMENTO</v>
       </c>
@@ -4744,24 +4703,24 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="54">
+        <v>12</v>
+      </c>
+      <c r="D20" s="27">
         <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="55" t="str">
+      <c r="A21" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-HOTELARIA</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="57">
+      <c r="C21" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="30">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correçao de erro de digitação
</commit_message>
<xml_diff>
--- a/SIMULADOR FII.xlsx
+++ b/SIMULADOR FII.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84704001185c0313/Documents/CURSO EXCEL/GIT-GITHUB-DIU/planilha-fiis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="8_{3FA65942-C9DF-468E-B0EA-5568C7E8B34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8427FD3E-3A8B-4AC6-B04A-C7AE871DC37A}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{3FA65942-C9DF-468E-B0EA-5568C7E8B34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B49C9EFC-A60E-447C-93AA-4C570460E46D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6EB58D97-D116-4FEE-B598-F6572D0553C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EB58D97-D116-4FEE-B598-F6572D0553C4}"/>
   </bookViews>
   <sheets>
     <sheet name="FIIs - Análise Investimeno" sheetId="1" r:id="rId1"/>
@@ -1067,18 +1067,84 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1089,72 +1155,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1561,22 +1561,22 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.05</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1844,22 +1844,22 @@
                 <c:formatCode>"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3701,6 +3701,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -4020,7 +4024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40130C33-4D69-4023-9FE0-85DE6757A8FE}">
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -4050,101 +4054,101 @@
     <row r="11" spans="4:6" x14ac:dyDescent="0.25"/>
     <row r="12" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="73"/>
-      <c r="F13" s="74"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
     </row>
     <row r="14" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="75"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="77"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="69"/>
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="84" t="s">
+      <c r="D15" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="85"/>
+      <c r="E15" s="77"/>
       <c r="F15" s="9">
         <v>4200</v>
       </c>
     </row>
     <row r="16" spans="4:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="59"/>
+      <c r="E16" s="79"/>
       <c r="F16" s="10">
         <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="57"/>
+      <c r="E17" s="81"/>
       <c r="F17" s="11">
         <f>F15*30%</f>
         <v>1260</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="59"/>
+      <c r="E18" s="79"/>
       <c r="F18" s="12">
         <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="59"/>
+      <c r="E19" s="79"/>
       <c r="F19" s="13">
         <v>5</v>
       </c>
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="61"/>
+      <c r="E20" s="83"/>
       <c r="F20" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D22" s="78" t="s">
+      <c r="D22" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="79"/>
-      <c r="F22" s="80"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="72"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="81"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="83"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="75"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D24" s="62" t="s">
+      <c r="D24" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="63"/>
+      <c r="E24" s="85"/>
       <c r="F24" s="15">
         <f>FV(tax_rendimento,prazo_anos*12,aporte)*-1</f>
         <v>114051.53941827051</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="65"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="16">
         <f>F24*tax_rendimento</f>
         <v>2281.03078836541</v>
@@ -4157,20 +4161,20 @@
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="68" t="s">
+      <c r="E28" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="70" t="s">
+      <c r="F28" s="62" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="67"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="71"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="63"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -4307,11 +4311,11 @@
       </c>
       <c r="E57" s="47">
         <f>VLOOKUP(perfil&amp;"-"&amp;D57,Perfis!$A:$D,4,)</f>
-        <v>0.5</v>
+        <v>0.32</v>
       </c>
       <c r="F57" s="48">
         <f>$E$55*E57</f>
-        <v>500</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.25">
@@ -4320,11 +4324,11 @@
       </c>
       <c r="E58" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D58,Perfis!$A:$D,4,)</f>
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="F58" s="48">
         <f t="shared" ref="F58:F62" si="0">$E$55*E58</f>
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.25">
@@ -4333,11 +4337,11 @@
       </c>
       <c r="E59" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D59,Perfis!$A:$D,4,)</f>
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="F59" s="48">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
@@ -4346,11 +4350,11 @@
       </c>
       <c r="E60" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D60,Perfis!$A:$D,4,)</f>
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F60" s="48">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.25">
@@ -4359,11 +4363,11 @@
       </c>
       <c r="E61" s="24">
         <f>VLOOKUP(perfil&amp;"-"&amp;D61,Perfis!$A:$D,4,)</f>
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F61" s="48">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4372,11 +4376,11 @@
       </c>
       <c r="E62" s="42">
         <f>VLOOKUP(perfil&amp;"-"&amp;D62,Perfis!$A:$D,4,)</f>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F62" s="55">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="4:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -4427,7 +4431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFA9F09-09B6-405B-A602-891185294CC5}">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>